<commit_message>
Add more sample data and improve researcher card layout
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="51">
   <si>
     <t>name</t>
   </si>
@@ -53,7 +53,7 @@
     <t>Visiting Scholar</t>
   </si>
   <si>
-    <t>Supports applied AI prototyping and research web tools.</t>
+    <t>Supports applied AI prototyping and research web tools focused on hospital operations.</t>
   </si>
   <si>
     <t>https://placehold.co/400x400/png?text=Diego</t>
@@ -62,6 +62,36 @@
     <t>diego-gonzalez-garcia-torres</t>
   </si>
   <si>
+    <t>Maya Singh</t>
+  </si>
+  <si>
+    <t>Data Scientist</t>
+  </si>
+  <si>
+    <t>Builds demand forecasting pipelines and evaluates model performance across hospital units.</t>
+  </si>
+  <si>
+    <t>https://placehold.co/400x400/png?text=Maya</t>
+  </si>
+  <si>
+    <t>maya-singh</t>
+  </si>
+  <si>
+    <t>Jordan Lee</t>
+  </si>
+  <si>
+    <t>Health Systems Engineer</t>
+  </si>
+  <si>
+    <t>Partners with clinical teams to translate analytics into staffing and workflow improvements.</t>
+  </si>
+  <si>
+    <t>https://placehold.co/400x400/png?text=Jordan</t>
+  </si>
+  <si>
+    <t>jordan-lee</t>
+  </si>
+  <si>
     <t>summary</t>
   </si>
   <si>
@@ -95,7 +125,49 @@
     <t>Operational decision support for system-wide challenges.|Forecasting demand and attrition to guide staffing and resources.|AI-driven insights to reduce burnout and turnover.</t>
   </si>
   <si>
-    <t>Overview::https://placehold.co/960x540/png?text=Slide+1::High-level overview|Challenges::https://placehold.co/960x540/png?text=Slide+2::Key system constraints</t>
+    <t>Overview::https://placehold.co/960x540/png?text=Predict+Slide+1::High-level overview|Challenges::https://placehold.co/960x540/png?text=Predict+Slide+2::Key system constraints</t>
+  </si>
+  <si>
+    <t>nursing-demand-forecast</t>
+  </si>
+  <si>
+    <t>Nursing Demand Forecast</t>
+  </si>
+  <si>
+    <t>Forecast nurse demand and optimize staffing plans across critical units.</t>
+  </si>
+  <si>
+    <t>https://placehold.co/900x600/png?text=Nursing+Demand+Forecast</t>
+  </si>
+  <si>
+    <t>Maya Singh::Data Scientist::maya-singh|Jordan Lee::Health Systems Engineer::jordan-lee</t>
+  </si>
+  <si>
+    <t>Integrates historical staffing and census data.|Produces 12-month forecasts by unit.|Flags high-risk gaps for mitigation planning.</t>
+  </si>
+  <si>
+    <t>Model Inputs::https://placehold.co/960x540/png?text=Demand+Slide+1::Historical and demographic signals|Results::https://placehold.co/960x540/png?text=Demand+Slide+2::Projected utilization curves</t>
+  </si>
+  <si>
+    <t>attrition-phenotyping</t>
+  </si>
+  <si>
+    <t>Attrition Phenotyping</t>
+  </si>
+  <si>
+    <t>Identify distinct attrition profiles and drivers across nursing populations.</t>
+  </si>
+  <si>
+    <t>https://placehold.co/900x600/png?text=Attrition+Phenotyping</t>
+  </si>
+  <si>
+    <t>Maya Singh::Data Scientist::maya-singh|Theofilos::Principal Investigator::theofilos</t>
+  </si>
+  <si>
+    <t>Clusters separations by role and tenure.|Combines well-being surveys with HR data.|Surfaces modifiable risk factors for intervention.</t>
+  </si>
+  <si>
+    <t>Cluster View::https://placehold.co/960x540/png?text=Attrition+Slide+1::Phenotype clusters|Interventions::https://placehold.co/960x540/png?text=Attrition+Slide+2::Mitigation strategies</t>
   </si>
 </sst>
 </file>
@@ -440,7 +512,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -497,10 +569,46 @@
         <v>14</v>
       </c>
     </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>
     <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="D4" r:id="rId3"/>
+    <hyperlink ref="D5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -508,7 +616,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -522,47 +630,95 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="D1" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="E1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="F1" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="G1" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="E2" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="F2" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="G2" t="s">
-        <v>26</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G4" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="D4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add PPTX presentations and publication linking
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -9,13 +9,14 @@
   <sheets>
     <sheet name="Researchers" sheetId="1" r:id="rId1"/>
     <sheet name="Projects" sheetId="2" r:id="rId2"/>
+    <sheet name="Publications" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="86">
   <si>
     <t>name</t>
   </si>
@@ -104,7 +105,7 @@
     <t>details</t>
   </si>
   <si>
-    <t>slides</t>
+    <t>presentations</t>
   </si>
   <si>
     <t>predict-operational-ai</t>
@@ -116,16 +117,13 @@
     <t>Decision support to provide enterprise insights and address health system-wide issues.</t>
   </si>
   <si>
-    <t>https://placehold.co/900x600/png?text=Predict+Operational+AI</t>
-  </si>
-  <si>
     <t>Theofilos::Principal Investigator::theofilos|Diego Gonzalez Garcia-Torres::Visiting Scholar::diego-gonzalez-garcia-torres</t>
   </si>
   <si>
     <t>Operational decision support for system-wide challenges.|Forecasting demand and attrition to guide staffing and resources.|AI-driven insights to reduce burnout and turnover.</t>
   </si>
   <si>
-    <t>Overview::https://placehold.co/960x540/png?text=Predict+Slide+1::High-level overview|Challenges::https://placehold.co/960x540/png?text=Predict+Slide+2::Key system constraints</t>
+    <t>Predict Overview::predict-overview.pptx::https://placehold.co/960x540/png?text=Predict+Deck+1|Predict Update::predict-update.pptx::https://placehold.co/960x540/png?text=Predict+Deck+2</t>
   </si>
   <si>
     <t>nursing-demand-forecast</t>
@@ -137,16 +135,13 @@
     <t>Forecast nurse demand and optimize staffing plans across critical units.</t>
   </si>
   <si>
-    <t>https://placehold.co/900x600/png?text=Nursing+Demand+Forecast</t>
-  </si>
-  <si>
     <t>Maya Singh::Data Scientist::maya-singh|Jordan Lee::Health Systems Engineer::jordan-lee</t>
   </si>
   <si>
     <t>Integrates historical staffing and census data.|Produces 12-month forecasts by unit.|Flags high-risk gaps for mitigation planning.</t>
   </si>
   <si>
-    <t>Model Inputs::https://placehold.co/960x540/png?text=Demand+Slide+1::Historical and demographic signals|Results::https://placehold.co/960x540/png?text=Demand+Slide+2::Projected utilization curves</t>
+    <t>Demand Forecast Brief::nursing-demand-brief.pptx::https://placehold.co/960x540/png?text=Demand+Deck+1</t>
   </si>
   <si>
     <t>attrition-phenotyping</t>
@@ -158,16 +153,127 @@
     <t>Identify distinct attrition profiles and drivers across nursing populations.</t>
   </si>
   <si>
-    <t>https://placehold.co/900x600/png?text=Attrition+Phenotyping</t>
-  </si>
-  <si>
     <t>Maya Singh::Data Scientist::maya-singh|Theofilos::Principal Investigator::theofilos</t>
   </si>
   <si>
     <t>Clusters separations by role and tenure.|Combines well-being surveys with HR data.|Surfaces modifiable risk factors for intervention.</t>
   </si>
   <si>
-    <t>Cluster View::https://placehold.co/960x540/png?text=Attrition+Slide+1::Phenotype clusters|Interventions::https://placehold.co/960x540/png?text=Attrition+Slide+2::Mitigation strategies</t>
+    <t>Attrition Insights::attrition-insights.pptx::https://placehold.co/960x540/png?text=Attrition+Deck+1</t>
+  </si>
+  <si>
+    <t>url</t>
+  </si>
+  <si>
+    <t>authors</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>project</t>
+  </si>
+  <si>
+    <t>researchers</t>
+  </si>
+  <si>
+    <t>operational-ai-in-practice</t>
+  </si>
+  <si>
+    <t>Operational AI in Practice</t>
+  </si>
+  <si>
+    <t>https://example.com/operational-ai</t>
+  </si>
+  <si>
+    <t>Theofilos, Diego Gonzalez Garcia-Torres</t>
+  </si>
+  <si>
+    <t>2024</t>
+  </si>
+  <si>
+    <t>theofilos|diego-gonzalez-garcia-torres</t>
+  </si>
+  <si>
+    <t>forecasting-nurse-demand</t>
+  </si>
+  <si>
+    <t>Forecasting Nurse Demand</t>
+  </si>
+  <si>
+    <t>https://example.com/nurse-demand</t>
+  </si>
+  <si>
+    <t>Maya Singh, Jordan Lee</t>
+  </si>
+  <si>
+    <t>2025</t>
+  </si>
+  <si>
+    <t>maya-singh|jordan-lee</t>
+  </si>
+  <si>
+    <t>attrition-phenotypes-at-scale</t>
+  </si>
+  <si>
+    <t>Attrition Phenotypes at Scale</t>
+  </si>
+  <si>
+    <t>https://example.com/attrition-phenotypes</t>
+  </si>
+  <si>
+    <t>Maya Singh, Theofilos</t>
+  </si>
+  <si>
+    <t>maya-singh|theofilos</t>
+  </si>
+  <si>
+    <t>operational-ai-decision-support</t>
+  </si>
+  <si>
+    <t>Operational AI Decision Support</t>
+  </si>
+  <si>
+    <t>https://example.com/decision-support</t>
+  </si>
+  <si>
+    <t>Theofilos, Jordan Lee</t>
+  </si>
+  <si>
+    <t>theofilos|jordan-lee</t>
+  </si>
+  <si>
+    <t>wellbeing-signals-in-staffing</t>
+  </si>
+  <si>
+    <t>Well-being Signals in Staffing</t>
+  </si>
+  <si>
+    <t>https://example.com/wellbeing-signals</t>
+  </si>
+  <si>
+    <t>Maya Singh, Diego Gonzalez Garcia-Torres</t>
+  </si>
+  <si>
+    <t>2023</t>
+  </si>
+  <si>
+    <t>maya-singh|diego-gonzalez-garcia-torres</t>
+  </si>
+  <si>
+    <t>systemwide-workforce-analytics</t>
+  </si>
+  <si>
+    <t>System-wide Workforce Analytics</t>
+  </si>
+  <si>
+    <t>https://example.com/workforce-analytics</t>
+  </si>
+  <si>
+    <t>Theofilos, Maya Singh</t>
+  </si>
+  <si>
+    <t>theofilos|maya-singh</t>
   </si>
 </sst>
 </file>
@@ -655,70 +761,232 @@
       <c r="C2" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" t="s">
         <v>33</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>34</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>35</v>
-      </c>
-      <c r="G2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" t="s">
         <v>37</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>38</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="F3" t="s">
         <v>40</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>41</v>
-      </c>
-      <c r="F3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G3" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" t="s">
         <v>44</v>
       </c>
+      <c r="E4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>65</v>
+      </c>
       <c r="B4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>47</v>
+        <v>66</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4" t="s">
+        <v>68</v>
       </c>
       <c r="E4" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="F4" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="G4" t="s">
-        <v>50</v>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E6" t="s">
+        <v>79</v>
+      </c>
+      <c r="G6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" t="s">
+        <v>84</v>
+      </c>
+      <c r="E7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G7" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
-    <hyperlink ref="D4" r:id="rId3"/>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="C5" r:id="rId4"/>
+    <hyperlink ref="C6" r:id="rId5"/>
+    <hyperlink ref="C7" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>